<commit_message>
file excel import change
</commit_message>
<xml_diff>
--- a/Templates/import_class.xlsx
+++ b/Templates/import_class.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kerss\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Пользователь\Documents\ACT\schoolServer\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11700" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11700" windowHeight="8328"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>1а</t>
-  </si>
-  <si>
-    <t>1б</t>
-  </si>
-  <si>
-    <t>1в</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Андреева</t>
   </si>
@@ -65,13 +56,19 @@
     <t>2 смена</t>
   </si>
   <si>
-    <t>12к12412</t>
-  </si>
-  <si>
-    <t>512е1252</t>
-  </si>
-  <si>
-    <t>12512у12</t>
+    <t>level</t>
+  </si>
+  <si>
+    <t>1к</t>
+  </si>
+  <si>
+    <t>5к</t>
+  </si>
+  <si>
+    <t>10к</t>
+  </si>
+  <si>
+    <t>1к24</t>
   </si>
 </sst>
 </file>
@@ -421,90 +418,102 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>